<commit_message>
02-03-2023 ->DPLKINV129-001, DPLKINV129-002, DPLKINV131-001, DPLKINV131-002, DPLKINV160-001, DPLKINV161-001, DPLKINV161-002, DPLKKPS119-001, DPLKKPS122-001, DPLKKPS135-001, DPLKKPS135-002, DPLKKPS136-002
03-03-2023
->DPLKKEU006-001,DPLKKEU028-001, DPLKKEU030-001, DPLKKEU031-001, DPLKKPS138-001 until DPLKKPS139-002

06-03-2023
->DPLKKEU008-001, DPLKKPS129-001 until DPLKKPS130-001, DPLKKPS143-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV129-001 until DPLKINV129 - Investasi - Fixed Income - Approve Dealing Ticket Fixed Income.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV129-001 until DPLKINV129 - Investasi - Fixed Income - Approve Dealing Ticket Fixed Income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF8505F-4509-4E9D-955F-C56FA3D5C7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5698A59-89D3-47F6-8186-3A1C4E8026EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKINV129-001" sheetId="3" r:id="rId1"/>
@@ -119,35 +119,35 @@
     <t>TICKET_ID</t>
   </si>
   <si>
+    <t>EXPLAIN</t>
+  </si>
+  <si>
+    <t>Diverifikasi</t>
+  </si>
+  <si>
+    <t>Dikembalikan Ke Register</t>
+  </si>
+  <si>
+    <t>DTOBL202300026</t>
+  </si>
+  <si>
     <t>Username : 33372;
 Password : bni1234;
 Role : 18 - Pimpinan Kelompok Investasi;
-Ticket ID : DTOBL202300024;
+Ticket ID : DTOBL202300026;
 Status Verifikasi : 1 : Setuju;
 Keterangan Verifikasi : INV.FIX.BEJ.011 DISETUJUI</t>
   </si>
   <si>
-    <t>EXPLAIN</t>
-  </si>
-  <si>
-    <t>Diverifikasi</t>
+    <t>DTOBL202300027</t>
   </si>
   <si>
     <t>Username : 33372;
 Password : bni1234;
 Role : 18 - Pimpinan Kelompok Investasi;
-Ticket ID : DTOBL202300022;
+Ticket ID : DTOBL202300027;
 Status Verifikasi : 0 : Kembalikan ke Data Entry;
 Keterangan Verifikasi : INV.FIX.BEJ.011 dikembalikan ke Data Entry</t>
-  </si>
-  <si>
-    <t>DTOBL202300022</t>
-  </si>
-  <si>
-    <t>Dikembalikan Ke Register</t>
-  </si>
-  <si>
-    <t>DTOBL202300019</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653A54F0-D01B-49C0-BB41-F0FC7D2164BA}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
         <v>17</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="102" x14ac:dyDescent="0.25">
@@ -640,7 +640,7 @@
         <v>24</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G2" s="3">
         <v>33372</v>
@@ -664,7 +664,7 @@
         <v>28</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
@@ -673,7 +673,7 @@
         <v>29</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X2" s="9"/>
       <c r="Y2" s="9"/>
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33B3AAE-605A-4DDB-BFFB-66C1AF414C99}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +787,7 @@
         <v>17</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="114.75" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3">
         <v>33372</v>
@@ -831,7 +831,7 @@
         <v>28</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
@@ -840,7 +840,7 @@
         <v>30</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="X2" s="9"/>
       <c r="Y2" s="9"/>

</xml_diff>